<commit_message>
Set up the system to run with Ollama
</commit_message>
<xml_diff>
--- a/data/intermediate/table2.02_20241202_e(2)_2.02 In Rupee SITC 2014-2024_organized.xlsx
+++ b/data/intermediate/table2.02_20241202_e(2)_2.02 In Rupee SITC 2014-2024_organized.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T325"/>
+  <dimension ref="A1:T158"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,7 +526,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>1900-01-13</t>
+          <t xml:space="preserve">                National Gem and Jewellery Authority</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -566,7 +566,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1900-01-21</t>
+          <t xml:space="preserve">               Central Bank of Sri Lanka</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -606,7 +606,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1903-12-18</t>
+          <t xml:space="preserve">               Sri Lanka Customs</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -646,7 +646,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1905-05-26</t>
+          <t>(a)  The latest version of SITC Revision 4 published in 2006</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -686,7 +686,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1909-06-19</t>
+          <t>(b) Provisional</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -726,7 +726,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1909-07-24</t>
+          <t>2.02: Export Performance based on Standard International Trade Classification (SITC) Monthly 2014-2024 (a)</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -766,7 +766,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1915-09-11</t>
+          <t>2.02: Export Performance based on Standard International Trade Classification (SITC) Monthly 2014-2024 (a)</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -806,7 +806,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1921-03-04</t>
+          <t>2023</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -846,7 +846,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1922-01-24</t>
+          <t>2024</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -886,7 +886,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1932-02-20</t>
+          <t>January</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -926,7 +926,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1938-09-27</t>
+          <t>January</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -966,7 +966,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1946-01-24</t>
+          <t>January</t>
         </is>
       </c>
       <c r="D13" t="n">
@@ -1006,14 +1006,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1954-11-18</t>
+          <t>January</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1975-07-04</t>
+          <t>January</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -1053,7 +1053,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>January</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1093,7 +1093,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>January</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -1133,7 +1133,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2023-01-01</t>
+          <t>January</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -1173,7 +1173,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2024-01-01</t>
+          <t>January</t>
         </is>
       </c>
       <c r="D19" t="n">
@@ -1213,7 +1213,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2024-01-01</t>
+          <t>January</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -1253,7 +1253,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2024-01-01</t>
+          <t>January</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1293,7 +1293,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2040-04-28</t>
+          <t>Sources: Ceylon Petroleum Corporation and Other Exporters of Petroleum</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1333,7 +1333,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2053-12-23</t>
+          <t>Table 2.02.4: Exports (Rs Million)</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1371,11 +1371,6 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>2085-08-13</t>
-        </is>
-      </c>
       <c r="D24" t="n">
         <v>119864.5898914578</v>
       </c>
@@ -1411,11 +1406,6 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>2107-07-26</t>
-        </is>
-      </c>
       <c r="D25" t="n">
         <v>119076.7354129021</v>
       </c>
@@ -1451,11 +1441,6 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>2255-02-09</t>
-        </is>
-      </c>
       <c r="D26" t="n">
         <v>117699.4591706567</v>
       </c>
@@ -1490,19 +1475,8 @@
         <v>0.281916</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>2346-10-16</t>
-        </is>
-      </c>
-    </row>
+    <row r="27"/>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>2753-08-02</t>
-        </is>
-      </c>
       <c r="D28" t="n">
         <v>129343.9789760905</v>
       </c>
@@ -1538,11 +1512,6 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>2870-08-11</t>
-        </is>
-      </c>
       <c r="D29" t="n">
         <v>128326.1328473097</v>
       </c>
@@ -1578,11 +1547,6 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                National Gem and Jewellery Authority</t>
-        </is>
-      </c>
       <c r="D30" t="n">
         <v>136619.1455796681</v>
       </c>
@@ -1618,11 +1582,6 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">               Central Bank of Sri Lanka</t>
-        </is>
-      </c>
       <c r="D31" t="n">
         <v>102225.1604335564</v>
       </c>
@@ -1658,11 +1617,6 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t xml:space="preserve">               Sri Lanka Customs</t>
-        </is>
-      </c>
       <c r="D32" t="n">
         <v>113625.6841330364</v>
       </c>
@@ -1698,11 +1652,6 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>(a)  The latest version of SITC Revision 4 published in 2006</t>
-        </is>
-      </c>
       <c r="D33" t="n">
         <v>130836.881528952</v>
       </c>
@@ -1738,11 +1687,6 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>(b) Provisional</t>
-        </is>
-      </c>
       <c r="D34" t="n">
         <v>129636.7333970337</v>
       </c>
@@ -1778,11 +1722,6 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2.02: Export Performance based on Standard International Trade Classification (SITC) Monthly 2014-2024 (a)</t>
-        </is>
-      </c>
       <c r="D35" t="n">
         <v>126135.5893405327</v>
       </c>
@@ -1818,11 +1757,6 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>2.02: Export Performance based on Standard International Trade Classification (SITC) Monthly 2014-2024 (a)</t>
-        </is>
-      </c>
       <c r="D36" t="n">
         <v>130896.9917660364</v>
       </c>
@@ -1858,11 +1792,6 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Animal and Vegetable Oils, Fats and Waxes</t>
-        </is>
-      </c>
       <c r="D37" t="n">
         <v>125582.1498270792</v>
       </c>
@@ -1898,11 +1827,6 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Animal and Vegetable Oils, Fats and Waxes</t>
-        </is>
-      </c>
       <c r="D38" t="n">
         <v>119642.8701244973</v>
       </c>
@@ -1938,11 +1862,6 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D39" t="n">
         <v>127894.3574199628</v>
       </c>
@@ -1977,19 +1896,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
-    </row>
+    <row r="40"/>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D41" t="n">
         <v>129789.444895598</v>
       </c>
@@ -2025,11 +1933,6 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D42" t="n">
         <v>130880.306814811</v>
       </c>
@@ -2065,11 +1968,6 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D43" t="n">
         <v>157759.9283618327</v>
       </c>
@@ -2105,11 +2003,6 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D44" t="n">
         <v>120597.5260285776</v>
       </c>
@@ -2145,11 +2038,6 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D45" t="n">
         <v>128150.5306206191</v>
       </c>
@@ -2185,11 +2073,6 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D46" t="n">
         <v>150890.2461416988</v>
       </c>
@@ -2225,11 +2108,6 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D47" t="n">
         <v>155998.9508570664</v>
       </c>
@@ -2265,11 +2143,6 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D48" t="n">
         <v>153291.4558362351</v>
       </c>
@@ -2305,11 +2178,6 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D49" t="n">
         <v>154583.177845383</v>
       </c>
@@ -2345,11 +2213,6 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D50" t="n">
         <v>149777.0617090051</v>
       </c>
@@ -2385,11 +2248,6 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D51" t="n">
         <v>144583.5187200061</v>
       </c>
@@ -2425,11 +2283,6 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D52" t="n">
         <v>156137.4829308398</v>
       </c>
@@ -2464,19 +2317,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
-    </row>
+    <row r="53"/>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D54" t="n">
         <v>148475.4725201858</v>
       </c>
@@ -2512,11 +2354,6 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D55" t="n">
         <v>141795.6896107451</v>
       </c>
@@ -2552,11 +2389,6 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D56" t="n">
         <v>172495.0704009031</v>
       </c>
@@ -2592,11 +2424,6 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D57" t="n">
         <v>124136.1791850057</v>
       </c>
@@ -2632,11 +2459,6 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D58" t="n">
         <v>145860.7754814224</v>
       </c>
@@ -2672,11 +2494,6 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D59" t="n">
         <v>162947.3898136775</v>
       </c>
@@ -2712,11 +2529,6 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
       <c r="D60" t="n">
         <v>170995.3167610536</v>
       </c>
@@ -2752,11 +2564,6 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D61" t="n">
         <v>166344.8201636997</v>
       </c>
@@ -2792,11 +2599,6 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D62" t="n">
         <v>173493.4263528746</v>
       </c>
@@ -2832,11 +2634,6 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D63" t="n">
         <v>167645.6300089614</v>
       </c>
@@ -2872,11 +2669,6 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D64" t="n">
         <v>173233.2380613535</v>
       </c>
@@ -2912,11 +2704,6 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D65" t="n">
         <v>186110.2310659289</v>
       </c>
@@ -2951,19 +2738,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
-    </row>
+    <row r="66"/>
     <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D67" t="n">
         <v>189075.2981964484</v>
       </c>
@@ -2999,11 +2775,6 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D68" t="n">
         <v>175358.5983049432</v>
       </c>
@@ -3039,11 +2810,6 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D69" t="n">
         <v>202850.1137905979</v>
       </c>
@@ -3079,11 +2845,6 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D70" t="n">
         <v>139509.8169983349</v>
       </c>
@@ -3119,11 +2880,6 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D71" t="n">
         <v>169566.8455475153</v>
       </c>
@@ -3159,11 +2915,6 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D72" t="n">
         <v>191414.3198787993</v>
       </c>
@@ -3199,11 +2950,6 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D73" t="n">
         <v>175732.2748641563</v>
       </c>
@@ -3239,11 +2985,6 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D74" t="n">
         <v>183755.4792060019</v>
       </c>
@@ -3279,11 +3020,6 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D75" t="n">
         <v>172415.1659485075</v>
       </c>
@@ -3319,11 +3055,6 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D76" t="n">
         <v>177328.5784216458</v>
       </c>
@@ -3359,11 +3090,6 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D77" t="n">
         <v>176546.4008792859</v>
       </c>
@@ -3399,11 +3125,6 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D78" t="n">
         <v>181243.5598038338</v>
       </c>
@@ -3438,19 +3159,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
-    </row>
+    <row r="79"/>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D80" t="n">
         <v>182289.7733871377</v>
       </c>
@@ -3486,11 +3196,6 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D81" t="n">
         <v>179477.9180216887</v>
       </c>
@@ -3526,11 +3231,6 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
       <c r="D82" t="n">
         <v>121437.6207454182</v>
       </c>
@@ -3566,11 +3266,6 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>Beverages and Tobacco</t>
-        </is>
-      </c>
       <c r="D83" t="n">
         <v>54510.00576392611</v>
       </c>
@@ -3606,11 +3301,6 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Beverages and Tobacco</t>
-        </is>
-      </c>
       <c r="D84" t="n">
         <v>110218.0047424168</v>
       </c>
@@ -3646,11 +3336,6 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>Central Bank of Sri Lanka</t>
-        </is>
-      </c>
       <c r="D85" t="n">
         <v>166268.482456108</v>
       </c>
@@ -3686,11 +3371,6 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Chemicals and Related Products, n.e.s.</t>
-        </is>
-      </c>
       <c r="D86" t="n">
         <v>201649.7561971526</v>
       </c>
@@ -3726,11 +3406,6 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>Chemicals and Related Products, n.e.s.</t>
-        </is>
-      </c>
       <c r="D87" t="n">
         <v>175136.7932178974</v>
       </c>
@@ -3766,11 +3441,6 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>Commodities and Transactions Not Classified Elsewhere in  the SITC</t>
-        </is>
-      </c>
       <c r="D88" t="n">
         <v>185039.4951275404</v>
       </c>
@@ -3806,11 +3476,6 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>Commodities and Transactions Not Classified Elsewhere in  the SITC</t>
-        </is>
-      </c>
       <c r="D89" t="n">
         <v>157560.7554383974</v>
       </c>
@@ -3846,11 +3511,6 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>Crude Materials, Inedible, except Fuels</t>
-        </is>
-      </c>
       <c r="D90" t="n">
         <v>144810.3714144285</v>
       </c>
@@ -3886,11 +3546,6 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>Crude Materials, Inedible, except Fuels</t>
-        </is>
-      </c>
       <c r="D91" t="n">
         <v>180528.0308229536</v>
       </c>
@@ -3925,19 +3580,8 @@
         <v>15.960937</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
-    </row>
+    <row r="92"/>
     <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D93" t="n">
         <v>178426.4839922678</v>
       </c>
@@ -3973,11 +3617,6 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D94" t="n">
         <v>184697.8570495727</v>
       </c>
@@ -4013,11 +3652,6 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D95" t="n">
         <v>215454.3078189924</v>
       </c>
@@ -4053,11 +3687,6 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D96" t="n">
         <v>161528.3912032979</v>
       </c>
@@ -4093,11 +3722,6 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D97" t="n">
         <v>177970.3196767834</v>
       </c>
@@ -4133,11 +3757,6 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D98" t="n">
         <v>201217.7502566961</v>
       </c>
@@ -4173,11 +3792,6 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D99" t="n">
         <v>220762.1785553684</v>
       </c>
@@ -4213,11 +3827,6 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D100" t="n">
         <v>220753.6387442055</v>
       </c>
@@ -4253,11 +3862,6 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D101" t="n">
         <v>208945.7306782832</v>
       </c>
@@ -4293,11 +3897,6 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D102" t="n">
         <v>239766.8153671478</v>
       </c>
@@ -4333,11 +3932,6 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D103" t="n">
         <v>244544.9662867</v>
       </c>
@@ -4373,11 +3967,6 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D104" t="n">
         <v>232874.3040198594</v>
       </c>
@@ -4412,19 +4001,8 @@
         <v>49.570283</v>
       </c>
     </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
-    </row>
+    <row r="105"/>
     <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D106" t="n">
         <v>222135.6767042945</v>
       </c>
@@ -4460,11 +4038,6 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D107" t="n">
         <v>220565.8205326789</v>
       </c>
@@ -4500,11 +4073,6 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D108" t="n">
         <v>270704.3283891963</v>
       </c>
@@ -4540,11 +4108,6 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D109" t="n">
         <v>310146.6153748021</v>
       </c>
@@ -4580,11 +4143,6 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D110" t="n">
         <v>376276.0260907023</v>
       </c>
@@ -4620,11 +4178,6 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
       <c r="D111" t="n">
         <v>449861.4311520494</v>
       </c>
@@ -4660,11 +4213,6 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D112" t="n">
         <v>420271.4719050966</v>
       </c>
@@ -4700,11 +4248,6 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D113" t="n">
         <v>442356.7087563006</v>
       </c>
@@ -4740,11 +4283,6 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D114" t="n">
         <v>391311.5661789599</v>
       </c>
@@ -4780,11 +4318,6 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D115" t="n">
         <v>381873.7294557405</v>
       </c>
@@ -4820,11 +4353,6 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D116" t="n">
         <v>361697.1958941522</v>
       </c>
@@ -4860,11 +4388,6 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D117" t="n">
         <v>387712.5684102305</v>
       </c>
@@ -4899,19 +4422,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
-    </row>
+    <row r="118"/>
     <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D119" t="n">
         <v>354510.8255109295</v>
       </c>
@@ -4947,11 +4459,6 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D120" t="n">
         <v>355446.6463585479</v>
       </c>
@@ -4987,11 +4494,6 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D121" t="n">
         <v>341811.1013812425</v>
       </c>
@@ -5027,11 +4529,6 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D122" t="n">
         <v>272764.1797953443</v>
       </c>
@@ -5067,11 +4564,6 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D123" t="n">
         <v>316208.4612653353</v>
       </c>
@@ -5107,11 +4599,6 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D124" t="n">
         <v>302870.8868704152</v>
       </c>
@@ -5147,11 +4634,6 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D125" t="n">
         <v>325815.5861104723</v>
       </c>
@@ -5187,11 +4669,6 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D126" t="n">
         <v>359729.8477633524</v>
       </c>
@@ -5227,11 +4704,6 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D127" t="n">
         <v>313702.4977548906</v>
       </c>
@@ -5267,11 +4739,6 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D128" t="n">
         <v>301336.5536737524</v>
       </c>
@@ -5307,11 +4774,6 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D129" t="n">
         <v>327912.7721568807</v>
       </c>
@@ -5347,11 +4809,6 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D130" t="n">
         <v>327317.4809205853</v>
       </c>
@@ -5386,19 +4843,8 @@
         <v>18.84298</v>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
-    </row>
+    <row r="131"/>
     <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D132" t="n">
         <v>311767.9966038866</v>
       </c>
@@ -5434,11 +4880,6 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
       <c r="D133" t="n">
         <v>331121.9021355574</v>
       </c>
@@ -5474,11 +4915,6 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>Food and Live Animals</t>
-        </is>
-      </c>
       <c r="D134" t="n">
         <v>351050.5084013312</v>
       </c>
@@ -5514,11 +4950,6 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>Food and Live Animals</t>
-        </is>
-      </c>
       <c r="D135" t="n">
         <v>262767.4343610767</v>
       </c>
@@ -5554,11 +4985,6 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
       <c r="D136" t="n">
         <v>303065.2450557924</v>
       </c>
@@ -5594,11 +5020,6 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
       <c r="D137" t="n">
         <v>327213.016527039</v>
       </c>
@@ -5634,11 +5055,6 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
       <c r="D138" t="n">
         <v>343329.0845274474</v>
       </c>
@@ -5674,11 +5090,6 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
       <c r="D139" t="n">
         <v>370327.7640660379</v>
       </c>
@@ -5714,11 +5125,6 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
       <c r="D140" t="n">
         <v>304685.1926357264</v>
       </c>
@@ -5754,11 +5160,6 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
       <c r="D141" t="n">
         <v>340202.6582398455</v>
       </c>
@@ -5793,1294 +5194,23 @@
         <v>8.134596</v>
       </c>
     </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="167">
-      <c r="A167" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="168">
-      <c r="A168" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="176">
-      <c r="A176" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="177">
-      <c r="A177" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-    </row>
-    <row r="178">
-      <c r="A178" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="179">
-      <c r="A179" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" t="inlineStr">
-        <is>
-          <t>Machinery and  Transport Equipment</t>
-        </is>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" t="inlineStr">
-        <is>
-          <t>Machinery and  Transport Equipment</t>
-        </is>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="inlineStr">
-        <is>
-          <t>Manufactured Goods Classified Chiefly by Material</t>
-        </is>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="inlineStr">
-        <is>
-          <t>Manufactured Goods Classified Chiefly by Material</t>
-        </is>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" t="inlineStr">
-        <is>
-          <t>Mineral Fuels, Lubricants and Related Materials</t>
-        </is>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" t="inlineStr">
-        <is>
-          <t>Mineral Fuels, Lubricants and Related Materials</t>
-        </is>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" t="inlineStr">
-        <is>
-          <t>Miscellaneous Manufactured Articles</t>
-        </is>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" t="inlineStr">
-        <is>
-          <t>Miscellaneous Manufactured Articles</t>
-        </is>
-      </c>
-    </row>
-    <row r="252">
-      <c r="A252" t="inlineStr">
-        <is>
-          <t>National Gem and Jewellery Authority</t>
-        </is>
-      </c>
-    </row>
-    <row r="253">
-      <c r="A253" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="254">
-      <c r="A254" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="255">
-      <c r="A255" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="256">
-      <c r="A256" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="257">
-      <c r="A257" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="258">
-      <c r="A258" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="259">
-      <c r="A259" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="260">
-      <c r="A260" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="261">
-      <c r="A261" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="262">
-      <c r="A262" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="263">
-      <c r="A263" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="264">
-      <c r="A264" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="265">
-      <c r="A265" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="266">
-      <c r="A266" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="267">
-      <c r="A267" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="268">
-      <c r="A268" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="269">
-      <c r="A269" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="270">
-      <c r="A270" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="271">
-      <c r="A271" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="272">
-      <c r="A272" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-    </row>
-    <row r="273">
-      <c r="A273" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="274">
-      <c r="A274" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="275">
-      <c r="A275" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="276">
-      <c r="A276" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="277">
-      <c r="A277" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="278">
-      <c r="A278" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="279">
-      <c r="A279" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="280">
-      <c r="A280" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="281">
-      <c r="A281" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="282">
-      <c r="A282" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="283">
-      <c r="A283" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="284">
-      <c r="A284" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="285">
-      <c r="A285" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="286">
-      <c r="A286" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="287">
-      <c r="A287" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="288">
-      <c r="A288" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="289">
-      <c r="A289" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="290">
-      <c r="A290" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="291">
-      <c r="A291" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="292">
-      <c r="A292" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="293">
-      <c r="A293" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="294">
-      <c r="A294" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-    </row>
-    <row r="295">
-      <c r="A295" t="inlineStr">
-        <is>
-          <t>Provisional</t>
-        </is>
-      </c>
-    </row>
-    <row r="296">
-      <c r="A296" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="297">
-      <c r="A297" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="298">
-      <c r="A298" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="299">
-      <c r="A299" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="300">
-      <c r="A300" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="301">
-      <c r="A301" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="302">
-      <c r="A302" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="303">
-      <c r="A303" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="304">
-      <c r="A304" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="305">
-      <c r="A305" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="306">
-      <c r="A306" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="307">
-      <c r="A307" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="308">
-      <c r="A308" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="309">
-      <c r="A309" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="310">
-      <c r="A310" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="311">
-      <c r="A311" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="312">
-      <c r="A312" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="313">
-      <c r="A313" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="314">
-      <c r="A314" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="315">
-      <c r="A315" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="316">
-      <c r="A316" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="317">
-      <c r="A317" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-    </row>
-    <row r="318">
-      <c r="A318" t="inlineStr">
-        <is>
-          <t>Sources: Ceylon Petroleum Corporation and Other Exporters of Petroleum</t>
-        </is>
-      </c>
-    </row>
-    <row r="319">
-      <c r="A319" t="inlineStr">
-        <is>
-          <t>Sources: Ceylon Petroleum Corporation and Other Exporters of Petroleum</t>
-        </is>
-      </c>
-    </row>
-    <row r="320">
-      <c r="A320" t="inlineStr">
-        <is>
-          <t>Sri Lanka Customs</t>
-        </is>
-      </c>
-    </row>
-    <row r="321">
-      <c r="A321" t="inlineStr">
-        <is>
-          <t>Table 2.02.4: Exports (Rs Million)</t>
-        </is>
-      </c>
-    </row>
-    <row r="322">
-      <c r="A322" t="inlineStr">
-        <is>
-          <t>Table 2.02.4: Exports (Rs Million)</t>
-        </is>
-      </c>
-    </row>
-    <row r="323">
-      <c r="A323" t="inlineStr">
-        <is>
-          <t>The latest version of SITC Revision 4 published in 2006</t>
-        </is>
-      </c>
-    </row>
-    <row r="324">
-      <c r="A324" t="inlineStr">
-        <is>
-          <t>Total Exports</t>
-        </is>
-      </c>
-    </row>
-    <row r="325">
-      <c r="A325" t="inlineStr">
-        <is>
-          <t>Total Exports</t>
-        </is>
-      </c>
-    </row>
+    <row r="142"/>
+    <row r="143"/>
+    <row r="144"/>
+    <row r="145"/>
+    <row r="146"/>
+    <row r="147"/>
+    <row r="148"/>
+    <row r="149"/>
+    <row r="150"/>
+    <row r="151"/>
+    <row r="152"/>
+    <row r="153"/>
+    <row r="154"/>
+    <row r="155"/>
+    <row r="156"/>
+    <row r="157"/>
+    <row r="158"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>